<commit_message>
added update and delete project
</commit_message>
<xml_diff>
--- a/backend/Controllers/public/student_data.xlsx
+++ b/backend/Controllers/public/student_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>S no.</t>
   </si>
@@ -37,25 +37,13 @@
     <t>Student 2 ID</t>
   </si>
   <si>
-    <t>aqsw</t>
-  </si>
-  <si>
-    <t>ANKIT GURWAN</t>
-  </si>
-  <si>
-    <t>210103016</t>
-  </si>
-  <si>
-    <t>a.gurwan@iitg.ac.in</t>
-  </si>
-  <si>
-    <t>Ankit Kumar</t>
-  </si>
-  <si>
-    <t>210103017</t>
-  </si>
-  <si>
-    <t>a.kumar@iitg.ac.in</t>
+    <t>wwaa</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>aa</t>
   </si>
 </sst>
 </file>
@@ -436,7 +424,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -485,19 +473,45 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added sign in with mircosoft
</commit_message>
<xml_diff>
--- a/backend/Controllers/public/student_data.xlsx
+++ b/backend/Controllers/public/student_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>S no.</t>
   </si>
@@ -35,27 +35,6 @@
   </si>
   <si>
     <t>Student 2 ID</t>
-  </si>
-  <si>
-    <t>aa</t>
-  </si>
-  <si>
-    <t>ANKIT GURWAN</t>
-  </si>
-  <si>
-    <t>210103016</t>
-  </si>
-  <si>
-    <t>a.gurwan@iitg.ac.in</t>
-  </si>
-  <si>
-    <t>HRISHI INANI</t>
-  </si>
-  <si>
-    <t>210103120</t>
-  </si>
-  <si>
-    <t>i.hrishi@iitg.ac.in</t>
   </si>
 </sst>
 </file>
@@ -436,7 +415,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -474,32 +453,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>